<commit_message>
fix(production_followup2.py): specify encoding when reading CSV file
docs(Report.csv): update production report data for January 2026

chore: add new Excel files for January 2026 reports
</commit_message>
<xml_diff>
--- a/Archive/2025/12. Dec/31-Dec-25.xlsx
+++ b/Archive/2025/12. Dec/31-Dec-25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\1. Daily\Production follow up\12. Dec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\1. Daily\Production follow up\Archive\2025\12. Dec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C0527D-3F02-45A6-BA27-F5B2E38E54CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80027971-2DC8-4CFD-9041-B9187698ED4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -626,7 +626,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,8 +1416,8 @@
         <v>732885</v>
       </c>
       <c r="C12" s="7">
-        <f>SUM(C4:C9)</f>
-        <v>16422890</v>
+        <f>SUM(C4:C11)</f>
+        <v>19759616</v>
       </c>
       <c r="D12" s="7">
         <v>18598707</v>
@@ -1531,7 +1531,7 @@
     <row r="16" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <f>C12</f>
-        <v>16422890</v>
+        <v>19759616</v>
       </c>
       <c r="B16" s="13">
         <f>D12</f>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="F16" s="13">
         <f t="shared" ref="F16:F21" si="13">$C$12-E16</f>
-        <v>-2175817</v>
+        <v>1160909</v>
       </c>
       <c r="M16" s="1"/>
     </row>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="F17" s="13">
         <f t="shared" si="13"/>
-        <v>-2175817</v>
+        <v>1160909</v>
       </c>
       <c r="M17" s="1"/>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="F18" s="13">
         <f t="shared" si="13"/>
-        <v>-2175817</v>
+        <v>1160909</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="F19" s="13">
         <f t="shared" si="13"/>
-        <v>-2175817</v>
+        <v>1160909</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="F20" s="13">
         <f t="shared" si="13"/>
-        <v>-2175817</v>
+        <v>1160909</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="F21" s="13">
         <f t="shared" si="13"/>
-        <v>-2175817</v>
+        <v>1160909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>